<commit_message>
updated flight computer documentation files/links
</commit_message>
<xml_diff>
--- a/SDR/A0002/BOM.xlsx
+++ b/SDR/A0002/BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="278">
   <si>
     <t>A0002 Flight Computer BOM</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0</t>
+    <t>2.0</t>
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
@@ -104,9 +104,8 @@
     <t>C0603C104J4RACTU</t>
   </si>
   <si>
-    <t>C2-C8, C17,
-C20-C21, 
-C23-C25</t>
+    <t>C2-C8, C17-C18,
+C20-C22, C24</t>
   </si>
   <si>
     <t>0603</t>
@@ -161,7 +160,10 @@
     <t>MCT06030C2400FP500</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>RC0603FR-07240RL</t>
   </si>
   <si>
     <t>2.2 uF 0603 Ceramic Capacitor</t>
@@ -173,7 +175,7 @@
     <t>CL10A225KO8NNNC</t>
   </si>
   <si>
-    <t>C12-C13</t>
+    <t>C11, C15</t>
   </si>
   <si>
     <t>1 uF 0603 Ceramic Capacitor</t>
@@ -182,7 +184,8 @@
     <t>C0603X105J4RACAUTO</t>
   </si>
   <si>
-    <t>C11, C16</t>
+    <t>C9, C23, 
+C25-C26</t>
   </si>
   <si>
     <t>10 uF Tantalum Capacitor</t>
@@ -191,7 +194,7 @@
     <t>T491A106K010AT</t>
   </si>
   <si>
-    <t>C14-C15</t>
+    <t>C10, C13</t>
   </si>
   <si>
     <t>Tactile Switch SMD</t>
@@ -218,12 +221,16 @@
     <t>SST25VF040B-50-4I-S2AE-T</t>
   </si>
   <si>
-    <t>U4</t>
+    <t>U6</t>
   </si>
   <si>
     <t>8-SOIC</t>
   </si>
   <si>
+    <t xml:space="preserve">        
+SST25VF040B-50-4I-S2AF-T</t>
+  </si>
+  <si>
     <t>IC USB-TO-UART BRIDGE 28VQFN</t>
   </si>
   <si>
@@ -233,7 +240,7 @@
     <t>CP2102-GMR</t>
   </si>
   <si>
-    <t>U3</t>
+    <t>U8</t>
   </si>
   <si>
     <t>QFN-28</t>
@@ -264,7 +271,7 @@
     <t>3220-20-0200-00</t>
   </si>
   <si>
-    <t>P8</t>
+    <t>P3</t>
   </si>
   <si>
     <t>20POS, 2ROW</t>
@@ -291,180 +298,181 @@
     <t>SP0504BAHTG</t>
   </si>
   <si>
-    <t>D6</t>
+    <t>D10</t>
   </si>
   <si>
     <t>SOT23-5</t>
   </si>
   <si>
-    <t>IGNITION SCREW TERMINALS</t>
+    <t>TERM BLK 6POS SIDE ENT 3.5MM PCB</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>6POS</t>
+  </si>
+  <si>
+    <t>E-match screw terminals</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
+  </si>
+  <si>
+    <t>R4-R5, 
+R31-R32</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>CL10A475KP8NNNC</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>280 Ohm Resistor 0603 SMD
+RGB LED current limiting Red</t>
+  </si>
+  <si>
+    <t>RMCF0603FT280R</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>82 Ohm Resistor 0603 SMD
+RGB LED current limiting Green</t>
+  </si>
+  <si>
+    <t>RMCF0603JT82R0</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+RMCF0603FT82R0</t>
+  </si>
+  <si>
+    <t>68 Ohm Resistor 0603 SMD
+RGB LED current limiting Blue</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>LED RGB CLEAR 4PLCC SMD</t>
+  </si>
+  <si>
+    <t>CreeLED, Inc.</t>
+  </si>
+  <si>
+    <t>CLMVC-FKA-CL1D1L71BB7C3C3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+  </si>
+  <si>
+    <t>R18, R19, R25</t>
+  </si>
+  <si>
+    <t>IC VOLT COMPARATOR SGL SOT-23-5</t>
+  </si>
+  <si>
+    <t>TS391IYLT</t>
+  </si>
+  <si>
+    <t>U9-U11</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>CRYSTAL 24.0000MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>ECS-240-18-33-JGN-TR</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>4-SMD, No Lead</t>
+  </si>
+  <si>
+    <t>CAP CER 8PF 250V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>CBR06C809BAGAC</t>
+  </si>
+  <si>
+    <t>C12, C14</t>
+  </si>
+  <si>
+    <t>TERM BLK 2POS SIDE ENT 3.5MM PCB</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>1546551-2</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>2POS</t>
+  </si>
+  <si>
+    <t>Main Power Connector</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 2POS 3.96MM</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP
+Connectors</t>
+  </si>
+  <si>
+    <t>647676-2</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>2POS, Right-Angle</t>
+  </si>
+  <si>
+    <t>CONN HOUSING 2POS .156" SNGL</t>
   </si>
   <si>
     <t>TE Connectivity AMP 
 Connectors</t>
   </si>
   <si>
-    <t>282837-6</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>6POS</t>
-  </si>
-  <si>
-    <t>through-hole</t>
-  </si>
-  <si>
-    <t>E-match screw terminals</t>
-  </si>
-  <si>
-    <t>RES 100K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics Inc</t>
-  </si>
-  <si>
-    <t>RMCF0603FT100K</t>
-  </si>
-  <si>
-    <t>R10-R13</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7UF 10V X5R 0603</t>
-  </si>
-  <si>
-    <t>CL10A475KP8NNNC</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>280 Ohm Resistor 0603 SMD
-RGB LED current limiting Red</t>
-  </si>
-  <si>
-    <t>RMCF0603FT280R</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>82 Ohm Resistor 0603 SMD
-RGB LED current limiting Green</t>
-  </si>
-  <si>
-    <t>RMCF0603JT82R0</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-RMCF0603FT82R0</t>
-  </si>
-  <si>
-    <t>68 Ohm Resistor 0603 SMD
-RGB LED current limiting Blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>LED RGB CLEAR 4PLCC SMD</t>
-  </si>
-  <si>
-    <t>CreeLED, Inc.</t>
-  </si>
-  <si>
-    <t>CLMVC-FKA-CL1D1L71BB7C3C3</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>RES 4.7K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RMCF0603FT4K70</t>
-  </si>
-  <si>
-    <t>R3, R29-R30</t>
-  </si>
-  <si>
-    <t>IC VOLT COMPARATOR SGL SOT-23-5</t>
-  </si>
-  <si>
-    <t>TS391IYLT</t>
-  </si>
-  <si>
-    <t>U5-U7</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>CRYSTAL 24.0000MHZ 18PF SMD</t>
-  </si>
-  <si>
-    <t>ECS Inc.</t>
-  </si>
-  <si>
-    <t>ECS-240-18-33-JGN-TR</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>4-SMD, No Lead</t>
-  </si>
-  <si>
-    <t>CAP CER 8PF 250V C0G/NP0 0603</t>
-  </si>
-  <si>
-    <t>CBR06C809BAGAC</t>
-  </si>
-  <si>
-    <t>C9-C10</t>
-  </si>
-  <si>
-    <t>TERM BLK 2P SIDE ENT 5.08MM PCB</t>
-  </si>
-  <si>
-    <t>282837-2</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>2POS</t>
-  </si>
-  <si>
-    <t>Main Power Connector</t>
-  </si>
-  <si>
-    <t>CONN HEADER R/A 2POS 3.96MM</t>
-  </si>
-  <si>
-    <t>TE Connectivity AMP
-Connectors</t>
-  </si>
-  <si>
-    <t>647676-2</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>2POS, Right-Angle</t>
-  </si>
-  <si>
-    <t>CONN HOUSING 2POS .156" SNGL</t>
-  </si>
-  <si>
     <t xml:space="preserve">	
 2132813-2</t>
   </si>
@@ -499,7 +507,7 @@
     <t>10118194-0001LF</t>
   </si>
   <si>
-    <t>P3</t>
+    <t>P8</t>
   </si>
   <si>
     <t>SMD/Through-hole</t>
@@ -514,9 +522,10 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>R5, R7-R10, 
-R14, R17-R20,
-R32</t>
+    <t>R7, R9, R20-R21, 
+R23-R24, R26,
+R28-R30, 
+R33-R36</t>
   </si>
   <si>
     <t>RES 1K OHM 1% 1/10W 0603</t>
@@ -525,28 +534,26 @@
     <t>RMCF0603FT1K00</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>IMU ACCEL/GYRO/MAG I2C/SPI 24QFN</t>
-  </si>
-  <si>
-    <t>CTR Electronics</t>
-  </si>
-  <si>
-    <t>MPU-9250</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>24QFN</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Registers</t>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>IMU ACCEL/GYRO I2C/SPI 14LGA</t>
+  </si>
+  <si>
+    <t>Bosch Sensortec</t>
+  </si>
+  <si>
+    <t>BMI323</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>14-VFLGA</t>
+  </si>
+  <si>
+    <t>Bosch 
+Sensortec</t>
   </si>
   <si>
     <t>BUZZER PIEZO 5V 13.8MM TH</t>
@@ -567,7 +574,7 @@
     <t>C0603X103F5JAC7867</t>
   </si>
   <si>
-    <t>C22, C26</t>
+    <t>C16</t>
   </si>
   <si>
     <t>RF RX GLONASS/GNSS/GPS 1.575GHZ</t>
@@ -579,7 +586,7 @@
     <t>MAX-8C-0</t>
   </si>
   <si>
-    <t>U9</t>
+    <t>U4</t>
   </si>
   <si>
     <t>18-SMD Module</t>
@@ -630,7 +637,7 @@
     <t>109990166/RFM95</t>
   </si>
   <si>
-    <t>U10</t>
+    <t>U7</t>
   </si>
   <si>
     <t>16-SMD Module</t>
@@ -661,22 +668,15 @@
     <t>SENSOR PRESSURE ABS</t>
   </si>
   <si>
-    <t>Bosch Sensortec</t>
-  </si>
-  <si>
     <t>BMP390</t>
   </si>
   <si>
-    <t>U11</t>
+    <t>U5</t>
   </si>
   <si>
     <t>10-WFLGA</t>
   </si>
   <si>
-    <t>Bosch 
-Sensortec</t>
-  </si>
-  <si>
     <t>RES 33 OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -686,19 +686,16 @@
     <t>RC0603FR-0733RL</t>
   </si>
   <si>
-    <t>R21-R28</t>
+    <t>R10-R17</t>
   </si>
   <si>
     <t>CONN HEADER VERT 3POS 2MM</t>
   </si>
   <si>
-    <t>TE Connectivity AMP Connectors</t>
-  </si>
-  <si>
     <t>440054-3</t>
   </si>
   <si>
-    <t>P5-P7, P9</t>
+    <t>P4-P7</t>
   </si>
   <si>
     <t>3POS</t>
@@ -734,7 +731,7 @@
     <t>MM3Z3V3B</t>
   </si>
   <si>
-    <t>D7-D10</t>
+    <t>D6-D9</t>
   </si>
   <si>
     <t>SOD-323F</t>
@@ -749,7 +746,7 @@
     <t>RC0603FR-0710RL</t>
   </si>
   <si>
-    <t>R31</t>
+    <t>R8</t>
   </si>
   <si>
     <t>FIXED IND 27NH 200MA 900MOHM SMD</t>
@@ -785,9 +782,33 @@
     <t>Drawing</t>
   </si>
   <si>
+    <t>RES 20K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-0720KL</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>SENSOR FLIPCORE/HALL SPI 12WLCSP</t>
+  </si>
+  <si>
+    <t>BMM150</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>12-WLCSP</t>
+  </si>
+  <si>
     <t>A0002 Flight Computer Production BOM</t>
   </si>
   <si>
+    <t>1.0</t>
+  </si>
+  <si>
     <t>01/23/2022</t>
   </si>
   <si>
@@ -809,35 +830,43 @@
     <t>Notes</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Sullins Connector Solutions</t>
-  </si>
-  <si>
-    <t>SBH11-PBPC-D05-RA-BK</t>
-  </si>
-  <si>
-    <t>Programming Connector: 10 pin 
-male header, right-angle</t>
-  </si>
-  <si>
-    <t>10POS, 2ROW</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>CWR11HH106KB</t>
-  </si>
-  <si>
-    <t>10 uF 2312 Tantalum Capacitor</t>
-  </si>
-  <si>
-    <t>2312</t>
+    <t>C2, C3, C4, C5, C6, C7, C8, C17, C18,
+C20, C21, C22, C24</t>
+  </si>
+  <si>
+    <t>C9, C23, 
+C25, C26</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6</t>
+  </si>
+  <si>
+    <t>R4, R5, 
+R31, R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>U9, U10, U11</t>
+  </si>
+  <si>
+    <t>D2, D3, D4</t>
+  </si>
+  <si>
+    <t>R7, R9, R20, R21, 
+R23, R24, R26,
+R28, R29, R30, 
+R33, R34, R35, R36</t>
+  </si>
+  <si>
+    <t>R10, R11, R12, R13, R14, R15, R16, R17</t>
+  </si>
+  <si>
+    <t>P4, P5, P6, P7</t>
+  </si>
+  <si>
+    <t>D6, D7, D8, D9</t>
   </si>
   <si>
     <t>AUTO-GENERATED</t>
@@ -852,7 +881,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="27">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -931,7 +960,34 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -954,7 +1010,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -971,12 +1027,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1072,7 +1122,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1204,50 +1254,83 @@
     <xf borderId="7" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="7" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="7" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="7" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1256,37 +1339,33 @@
     <xf borderId="7" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf quotePrefix="1" borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf quotePrefix="1" borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1504,16 +1583,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7.0" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B9" sqref="B9" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.13"/>
-    <col customWidth="1" min="2" max="2" width="36.13"/>
+    <col customWidth="1" min="2" max="2" width="36.25"/>
     <col customWidth="1" min="3" max="3" width="28.13"/>
-    <col customWidth="1" min="4" max="4" width="30.75"/>
+    <col customWidth="1" min="4" max="4" width="23.63"/>
+    <col customWidth="1" min="5" max="5" width="14.38"/>
     <col customWidth="1" min="6" max="6" width="15.25"/>
     <col customWidth="1" min="7" max="7" width="16.63"/>
     <col customWidth="1" min="9" max="9" width="25.0"/>
@@ -1592,7 +1676,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="12">
-        <v>44390.0</v>
+        <v>44903.0</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1697,7 +1781,7 @@
     </row>
     <row r="9">
       <c r="A9" s="23">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>27</v>
@@ -1830,7 +1914,9 @@
       <c r="J12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="7"/>
+      <c r="K12" s="33" t="s">
+        <v>49</v>
+      </c>
       <c r="L12" s="7"/>
     </row>
     <row r="13">
@@ -1838,16 +1924,16 @@
         <v>2.0</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="44" t="s">
         <v>31</v>
@@ -1859,7 +1945,7 @@
         <v>0.1</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>44</v>
@@ -1869,19 +1955,19 @@
     </row>
     <row r="14">
       <c r="A14" s="33">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>31</v>
@@ -1893,7 +1979,7 @@
         <v>0.48</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J14" s="38" t="s">
         <v>44</v>
@@ -1906,16 +1992,16 @@
         <v>2.0</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F15" s="44" t="s">
         <v>37</v>
@@ -1927,7 +2013,7 @@
         <v>0.37</v>
       </c>
       <c r="I15" s="43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J15" s="30" t="s">
         <v>44</v>
@@ -1940,19 +2026,19 @@
         <v>1.0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="36" t="s">
         <v>25</v>
@@ -1961,7 +2047,7 @@
         <v>0.18</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J16" s="38" t="s">
         <v>44</v>
@@ -1974,19 +2060,19 @@
         <v>1.0</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" s="44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>25</v>
@@ -1995,12 +2081,14 @@
         <v>0.92</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="23" t="s">
+        <v>70</v>
+      </c>
       <c r="L17" s="32"/>
     </row>
     <row r="18">
@@ -2008,19 +2096,19 @@
         <v>1.0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G18" s="36" t="s">
         <v>25</v>
@@ -2029,7 +2117,7 @@
         <v>3.24</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>26</v>
@@ -2038,23 +2126,23 @@
       <c r="L18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="32">
-        <v>1.0</v>
+      <c r="A19" s="23">
+        <v>6.0</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F19" s="44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>25</v>
@@ -2063,7 +2151,7 @@
         <v>0.63</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J19" s="30" t="s">
         <v>32</v>
@@ -2076,28 +2164,28 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H20" s="36">
         <v>1.43</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>44</v>
@@ -2110,13 +2198,13 @@
         <v>1.0</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="47"/>
@@ -2125,10 +2213,10 @@
         <v>25.31</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
@@ -2138,19 +2226,19 @@
         <v>1.0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G22" s="36" t="s">
         <v>25</v>
@@ -2159,7 +2247,7 @@
         <v>0.95</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J22" s="38" t="s">
         <v>44</v>
@@ -2168,37 +2256,37 @@
       <c r="L22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="32" t="s">
+      <c r="A23" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B23" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="C23" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="D23" s="50">
+        <v>1984659.0</v>
+      </c>
+      <c r="E23" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="F23" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="42">
-        <v>3.59</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="32"/>
+      <c r="G23" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="53">
+        <v>1.76</v>
+      </c>
+      <c r="I23" s="54">
+        <v>1984659.0</v>
+      </c>
+      <c r="J23" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="56"/>
       <c r="L23" s="23" t="s">
         <v>99</v>
       </c>
@@ -2234,7 +2322,9 @@
       <c r="J24" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="7"/>
+      <c r="K24" s="33" t="s">
+        <v>104</v>
+      </c>
       <c r="L24" s="7"/>
     </row>
     <row r="25">
@@ -2242,16 +2332,16 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F25" s="44" t="s">
         <v>31</v>
@@ -2263,7 +2353,7 @@
         <v>0.1</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J25" s="30" t="s">
         <v>44</v>
@@ -2272,20 +2362,20 @@
       <c r="L25" s="32"/>
     </row>
     <row r="26">
-      <c r="A26" s="49">
+      <c r="A26" s="57">
         <v>1.0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F26" s="35" t="s">
         <v>31</v>
@@ -2297,7 +2387,7 @@
         <v>0.1</v>
       </c>
       <c r="I26" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J26" s="38" t="s">
         <v>32</v>
@@ -2310,16 +2400,16 @@
         <v>1.0</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>101</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F27" s="44" t="s">
         <v>31</v>
@@ -2331,13 +2421,13 @@
         <v>0.1</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>32</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L27" s="32"/>
     </row>
@@ -2346,13 +2436,13 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>115</v>
+      <c r="D28" s="58" t="s">
+        <v>109</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>116</v>
@@ -2367,7 +2457,7 @@
         <v>0.1</v>
       </c>
       <c r="I28" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J28" s="38" t="s">
         <v>32</v>
@@ -2408,8 +2498,8 @@
       <c r="L29" s="32"/>
     </row>
     <row r="30">
-      <c r="A30" s="7">
-        <v>1.0</v>
+      <c r="A30" s="33">
+        <v>3.0</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>121</v>
@@ -2420,7 +2510,7 @@
       <c r="D30" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="59" t="s">
         <v>123</v>
       </c>
       <c r="F30" s="35" t="s">
@@ -2442,8 +2532,8 @@
       <c r="L30" s="7"/>
     </row>
     <row r="31">
-      <c r="A31" s="32">
-        <v>1.0</v>
+      <c r="A31" s="23">
+        <v>3.0</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>124</v>
@@ -2482,7 +2572,7 @@
       <c r="B32" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="60" t="s">
         <v>129</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -2544,75 +2634,75 @@
       <c r="L33" s="32"/>
     </row>
     <row r="34">
-      <c r="A34" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="B34" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="C34" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="D34" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="E34" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="G34" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" s="36">
-        <v>1.17</v>
-      </c>
-      <c r="I34" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="J34" s="38" t="s">
+      <c r="F34" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="64">
+        <v>1.34</v>
+      </c>
+      <c r="I34" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="J34" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="7"/>
+      <c r="K34" s="33"/>
       <c r="L34" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="51">
+      <c r="A35" s="66">
         <v>1.0</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F35" s="44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H35" s="42">
         <v>0.27</v>
       </c>
       <c r="I35" s="30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>44</v>
       </c>
       <c r="K35" s="32"/>
       <c r="L35" s="32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36">
@@ -2620,22 +2710,22 @@
         <v>1.0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="36">
         <v>0.27</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J36" s="38" t="s">
         <v>44</v>
@@ -2648,13 +2738,13 @@
         <v>2.0</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E37" s="32"/>
       <c r="F37" s="47"/>
@@ -2663,7 +2753,7 @@
         <v>0.18</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J37" s="30" t="s">
         <v>44</v>
@@ -2676,19 +2766,19 @@
         <v>3.0</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G38" s="36" t="s">
         <v>25</v>
@@ -2697,7 +2787,7 @@
         <v>0.35</v>
       </c>
       <c r="I38" s="38" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J38" s="38" t="s">
         <v>44</v>
@@ -2706,54 +2796,54 @@
       <c r="L38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B39" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D39" s="53" t="s">
+      <c r="A39" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B39" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="54" t="s">
+      <c r="C39" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="F39" s="53" t="s">
+      <c r="D39" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="G39" s="55" t="s">
+      <c r="E39" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="G39" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" s="53">
+        <v>0.48</v>
+      </c>
+      <c r="I39" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="H39" s="56">
-        <v>0.48</v>
-      </c>
-      <c r="I39" s="57" t="s">
-        <v>157</v>
-      </c>
-      <c r="J39" s="57" t="s">
+      <c r="J39" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
     </row>
     <row r="40">
       <c r="A40" s="33">
-        <v>11.0</v>
+        <v>14.0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E40" s="34" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F40" s="35" t="s">
         <v>31</v>
@@ -2765,7 +2855,7 @@
         <v>0.1</v>
       </c>
       <c r="I40" s="38" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J40" s="38" t="s">
         <v>32</v>
@@ -2778,16 +2868,16 @@
         <v>1.0</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C41" s="32" t="s">
         <v>101</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F41" s="44" t="s">
         <v>31</v>
@@ -2799,7 +2889,7 @@
         <v>0.1</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J41" s="30" t="s">
         <v>44</v>
@@ -2812,86 +2902,84 @@
         <v>1.0</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="F42" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="20">
+        <v>6.23</v>
+      </c>
+      <c r="I42" s="70" t="s">
         <v>171</v>
       </c>
-      <c r="G42" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="H42" s="20">
-        <v>10.0</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>172</v>
+      <c r="J42" s="70" t="s">
+        <v>174</v>
       </c>
       <c r="K42" s="22"/>
-      <c r="L42" s="21" t="s">
-        <v>173</v>
-      </c>
+      <c r="L42" s="71"/>
     </row>
     <row r="43">
-      <c r="A43" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="53" t="s">
+      <c r="A43" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B43" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="53" t="s">
+      <c r="C43" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="F43" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="H43" s="56">
+      <c r="E43" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="H43" s="53">
         <v>1.69</v>
       </c>
-      <c r="I43" s="57" t="s">
-        <v>176</v>
-      </c>
-      <c r="J43" s="57" t="s">
+      <c r="I43" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="J43" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
     </row>
     <row r="44">
       <c r="A44" s="33">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F44" s="35" t="s">
         <v>31</v>
@@ -2903,7 +2991,7 @@
         <v>0.94</v>
       </c>
       <c r="I44" s="38" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J44" s="38" t="s">
         <v>44</v>
@@ -2912,39 +3000,39 @@
       <c r="L44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B45" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="C45" s="53" t="s">
+      <c r="A45" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B45" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="C45" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="D45" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="F45" s="55" t="s">
+      <c r="E45" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H45" s="60">
+      <c r="F45" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="72">
         <v>21.0</v>
       </c>
-      <c r="I45" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="J45" s="57" t="s">
+      <c r="I45" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="J45" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="58"/>
-      <c r="L45" s="53" t="s">
-        <v>186</v>
+      <c r="K45" s="56"/>
+      <c r="L45" s="49" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="46">
@@ -2952,27 +3040,27 @@
         <v>1.0</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D46" s="61">
+        <v>189</v>
+      </c>
+      <c r="D46" s="73">
         <v>7.3412011E8</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="G46" s="59" t="s">
+      <c r="F46" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" s="69" t="s">
         <v>25</v>
       </c>
       <c r="H46" s="20">
         <v>0.77</v>
       </c>
-      <c r="I46" s="62">
+      <c r="I46" s="74">
         <v>7.3412011E8</v>
       </c>
       <c r="J46" s="21" t="s">
@@ -2980,43 +3068,43 @@
       </c>
       <c r="K46" s="22"/>
       <c r="L46" s="16" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B47" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="53" t="s">
+      <c r="A47" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B47" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="D47" s="63" t="s">
+      <c r="C47" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="D47" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="F47" s="55" t="s">
+      <c r="E47" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="G47" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H47" s="56">
+      <c r="F47" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="53">
         <v>1.99</v>
       </c>
-      <c r="I47" s="64" t="s">
-        <v>194</v>
-      </c>
-      <c r="J47" s="57" t="s">
+      <c r="I47" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="J47" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="K47" s="58"/>
-      <c r="L47" s="53" t="s">
-        <v>197</v>
+      <c r="K47" s="56"/>
+      <c r="L47" s="49" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="48">
@@ -3024,67 +3112,67 @@
         <v>1.0</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="D48" s="61" t="s">
         <v>200</v>
       </c>
+      <c r="D48" s="73" t="s">
+        <v>201</v>
+      </c>
       <c r="E48" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="F48" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="G48" s="59" t="s">
+      <c r="F48" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="G48" s="69" t="s">
         <v>25</v>
       </c>
       <c r="H48" s="20">
         <v>8.12</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J48" s="21" t="s">
         <v>44</v>
       </c>
       <c r="K48" s="22"/>
       <c r="L48" s="16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="65">
-        <v>1.0</v>
-      </c>
-      <c r="B49" s="66" t="s">
-        <v>205</v>
-      </c>
-      <c r="C49" s="66" t="s">
+      <c r="A49" s="76">
+        <v>1.0</v>
+      </c>
+      <c r="B49" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="C49" s="77" t="s">
         <v>207</v>
       </c>
+      <c r="D49" s="77" t="s">
+        <v>208</v>
+      </c>
       <c r="E49" s="39" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F49" s="47"/>
       <c r="G49" s="47"/>
       <c r="H49" s="42">
         <v>4.23</v>
       </c>
-      <c r="I49" s="67" t="s">
-        <v>207</v>
-      </c>
-      <c r="J49" s="67" t="s">
+      <c r="I49" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="J49" s="78" t="s">
         <v>44</v>
       </c>
       <c r="K49" s="32"/>
       <c r="L49" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50">
@@ -3092,10 +3180,10 @@
         <v>1.0</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>212</v>
@@ -3103,10 +3191,10 @@
       <c r="E50" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="F50" s="59" t="s">
+      <c r="F50" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="G50" s="59" t="s">
+      <c r="G50" s="69" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="20">
@@ -3116,109 +3204,109 @@
         <v>212</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
     </row>
     <row r="51">
-      <c r="A51" s="53">
+      <c r="A51" s="49">
         <v>8.0</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="C51" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="C51" s="53" t="s">
+      <c r="D51" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="D51" s="53" t="s">
+      <c r="E51" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="E51" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="F51" s="68" t="s">
+      <c r="F51" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H51" s="56">
+      <c r="G51" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="53">
         <v>0.1</v>
       </c>
-      <c r="I51" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="J51" s="57" t="s">
+      <c r="I51" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="J51" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
     </row>
     <row r="52">
       <c r="A52" s="16">
         <v>4.0</v>
       </c>
       <c r="B52" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="E52" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="F52" s="69" t="s">
         <v>222</v>
       </c>
-      <c r="E52" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="F52" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="G52" s="59" t="s">
-        <v>84</v>
+      <c r="G52" s="69" t="s">
+        <v>86</v>
       </c>
       <c r="H52" s="20">
         <v>0.27</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J52" s="21" t="s">
         <v>32</v>
       </c>
       <c r="K52" s="22"/>
       <c r="L52" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="49" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="53">
-        <v>4.0</v>
-      </c>
-      <c r="B53" s="53" t="s">
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="53">
+        <v>0.19</v>
+      </c>
+      <c r="I53" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="J53" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="K53" s="56"/>
+      <c r="L53" s="49" t="s">
         <v>226</v>
-      </c>
-      <c r="C53" s="53" t="s">
-        <v>221</v>
-      </c>
-      <c r="D53" s="53" t="s">
-        <v>227</v>
-      </c>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="56">
-        <v>0.19</v>
-      </c>
-      <c r="I53" s="53" t="s">
-        <v>227</v>
-      </c>
-      <c r="J53" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="K53" s="58"/>
-      <c r="L53" s="53" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="54">
@@ -3226,13 +3314,13 @@
         <v>12.0</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -3241,50 +3329,50 @@
         <v>0.01</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J54" s="21" t="s">
         <v>32</v>
       </c>
       <c r="K54" s="22"/>
       <c r="L54" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="C55" s="49" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="53">
-        <v>4.0</v>
-      </c>
-      <c r="B55" s="53" t="s">
+      <c r="D55" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="C55" s="53" t="s">
+      <c r="E55" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="D55" s="53" t="s">
+      <c r="F55" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="E55" s="54" t="s">
+      <c r="G55" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="I55" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="J55" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="K55" s="56"/>
+      <c r="L55" s="49" t="s">
         <v>235</v>
-      </c>
-      <c r="F55" s="55" t="s">
-        <v>236</v>
-      </c>
-      <c r="G55" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H55" s="56">
-        <v>0.25</v>
-      </c>
-      <c r="I55" s="57" t="s">
-        <v>234</v>
-      </c>
-      <c r="J55" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="K55" s="58"/>
-      <c r="L55" s="53" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="56">
@@ -3292,28 +3380,28 @@
         <v>1.0</v>
       </c>
       <c r="B56" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E56" s="17" t="s">
         <v>238</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>240</v>
       </c>
       <c r="F56" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G56" s="59" t="s">
+      <c r="G56" s="69" t="s">
         <v>25</v>
       </c>
       <c r="H56" s="20">
         <v>0.1</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J56" s="21" t="s">
         <v>44</v>
@@ -3322,57 +3410,57 @@
       <c r="L56" s="22"/>
     </row>
     <row r="57">
-      <c r="A57" s="53">
-        <v>1.0</v>
-      </c>
-      <c r="B57" s="53" t="s">
+      <c r="A57" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B57" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="C57" s="53" t="s">
+      <c r="E57" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="D57" s="53" t="s">
+      <c r="F57" s="79" t="s">
         <v>243</v>
       </c>
-      <c r="E57" s="54" t="s">
-        <v>244</v>
-      </c>
-      <c r="F57" s="68" t="s">
-        <v>245</v>
-      </c>
-      <c r="G57" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="56">
+      <c r="G57" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="53">
         <v>0.1</v>
       </c>
-      <c r="I57" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="J57" s="57" t="s">
+      <c r="I57" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="J57" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="K57" s="58"/>
-      <c r="L57" s="58"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
     </row>
     <row r="58">
       <c r="A58" s="7">
         <v>1.0</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="E58" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="F58" s="35" t="s">
         <v>248</v>
-      </c>
-      <c r="E58" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="F58" s="35" t="s">
-        <v>250</v>
       </c>
       <c r="G58" s="36" t="s">
         <v>25</v>
@@ -3381,15 +3469,97 @@
         <v>1.98</v>
       </c>
       <c r="I58" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J58" s="38" t="s">
         <v>44</v>
       </c>
       <c r="K58" s="7"/>
       <c r="L58" s="38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="B59" s="49" t="s">
+        <v>250</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" s="49" t="s">
         <v>251</v>
       </c>
+      <c r="E59" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="F59" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="I59" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="J59" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="K59" s="56"/>
+      <c r="L59" s="56"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F60" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="G60" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="20">
+        <v>2.34</v>
+      </c>
+      <c r="I60" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="J60" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+    </row>
+    <row r="61">
+      <c r="D61" s="80"/>
+      <c r="F61" s="81"/>
+      <c r="G61" s="81"/>
+      <c r="H61" s="82"/>
+      <c r="I61" s="80"/>
+      <c r="J61" s="83"/>
+    </row>
+    <row r="62">
+      <c r="F62" s="81"/>
+      <c r="G62" s="81"/>
+      <c r="H62" s="82"/>
+      <c r="J62" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3439,32 +3609,32 @@
     <hyperlink r:id="rId37" ref="J26"/>
     <hyperlink r:id="rId38" ref="I27"/>
     <hyperlink r:id="rId39" ref="J27"/>
-    <hyperlink r:id="rId40" ref="I28"/>
-    <hyperlink r:id="rId41" ref="J28"/>
-    <hyperlink r:id="rId42" ref="I29"/>
-    <hyperlink r:id="rId43" ref="J29"/>
-    <hyperlink r:id="rId44" ref="J30"/>
-    <hyperlink r:id="rId45" ref="I31"/>
-    <hyperlink r:id="rId46" ref="J31"/>
-    <hyperlink r:id="rId47" ref="I32"/>
-    <hyperlink r:id="rId48" ref="J32"/>
-    <hyperlink r:id="rId49" ref="J33"/>
-    <hyperlink r:id="rId50" ref="I34"/>
-    <hyperlink r:id="rId51" ref="J34"/>
-    <hyperlink r:id="rId52" ref="I35"/>
-    <hyperlink r:id="rId53" ref="J35"/>
-    <hyperlink r:id="rId54" ref="J36"/>
-    <hyperlink r:id="rId55" ref="J37"/>
-    <hyperlink r:id="rId56" ref="I38"/>
-    <hyperlink r:id="rId57" ref="J38"/>
-    <hyperlink r:id="rId58" ref="I39"/>
-    <hyperlink r:id="rId59" ref="J39"/>
-    <hyperlink r:id="rId60" ref="I40"/>
-    <hyperlink r:id="rId61" ref="J40"/>
-    <hyperlink r:id="rId62" ref="J41"/>
-    <hyperlink r:id="rId63" ref="I42"/>
-    <hyperlink r:id="rId64" ref="J42"/>
-    <hyperlink r:id="rId65" ref="L42"/>
+    <hyperlink r:id="rId40" ref="D28"/>
+    <hyperlink r:id="rId41" ref="I28"/>
+    <hyperlink r:id="rId42" ref="J28"/>
+    <hyperlink r:id="rId43" ref="I29"/>
+    <hyperlink r:id="rId44" ref="J29"/>
+    <hyperlink r:id="rId45" ref="J30"/>
+    <hyperlink r:id="rId46" ref="I31"/>
+    <hyperlink r:id="rId47" ref="J31"/>
+    <hyperlink r:id="rId48" ref="I32"/>
+    <hyperlink r:id="rId49" ref="J32"/>
+    <hyperlink r:id="rId50" ref="J33"/>
+    <hyperlink r:id="rId51" ref="I34"/>
+    <hyperlink r:id="rId52" ref="J34"/>
+    <hyperlink r:id="rId53" ref="I35"/>
+    <hyperlink r:id="rId54" ref="J35"/>
+    <hyperlink r:id="rId55" ref="J36"/>
+    <hyperlink r:id="rId56" ref="J37"/>
+    <hyperlink r:id="rId57" ref="I38"/>
+    <hyperlink r:id="rId58" ref="J38"/>
+    <hyperlink r:id="rId59" ref="I39"/>
+    <hyperlink r:id="rId60" ref="J39"/>
+    <hyperlink r:id="rId61" ref="I40"/>
+    <hyperlink r:id="rId62" ref="J40"/>
+    <hyperlink r:id="rId63" ref="J41"/>
+    <hyperlink r:id="rId64" ref="I42"/>
+    <hyperlink r:id="rId65" location="order" ref="J42"/>
     <hyperlink r:id="rId66" ref="I43"/>
     <hyperlink r:id="rId67" ref="J43"/>
     <hyperlink r:id="rId68" ref="I44"/>
@@ -3492,8 +3662,14 @@
     <hyperlink r:id="rId90" ref="I58"/>
     <hyperlink r:id="rId91" ref="J58"/>
     <hyperlink r:id="rId92" ref="L58"/>
+    <hyperlink r:id="rId93" ref="J59"/>
+    <hyperlink r:id="rId94" ref="I60"/>
+    <hyperlink r:id="rId95" ref="J60"/>
   </hyperlinks>
-  <drawing r:id="rId93"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <drawing r:id="rId96"/>
 </worksheet>
 </file>
 
@@ -3506,10 +3682,17 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="18.25"/>
+    <col customWidth="1" min="4" max="4" width="25.75"/>
+    <col customWidth="1" min="5" max="5" width="25.5"/>
+    <col customWidth="1" min="6" max="6" width="35.75"/>
+    <col customWidth="1" min="9" max="9" width="25.13"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="69" t="s">
-        <v>252</v>
+      <c r="A1" s="84" t="s">
+        <v>257</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3532,10 +3715,10 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="9"/>
@@ -3547,11 +3730,11 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
-        <v>4</v>
+      <c r="B4" s="86" t="s">
+        <v>258</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -3562,11 +3745,11 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="71" t="s">
-        <v>253</v>
+      <c r="B5" s="86" t="s">
+        <v>259</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -3577,10 +3760,10 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="85" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="9"/>
@@ -3592,172 +3775,1432 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="49" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>264</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="23">
+        <v>15.0</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="33">
+        <v>7.0</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="23">
+        <v>8.0</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="16">
+        <v>9.0</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="23">
+        <v>10.0</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="33">
+        <v>11.0</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="23">
+        <v>12.0</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="23">
+        <v>6.0</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="16">
+        <v>13.0</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="23">
+        <v>14.0</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="33">
+        <v>15.0</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="23">
+        <v>16.0</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="50">
+        <v>1984659.0</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="16">
+        <v>17.0</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="C24" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="23">
+        <v>18.0</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="33">
+        <v>19.0</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="57">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="23">
+        <v>20.0</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="16">
+        <v>21.0</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="23">
+        <v>22.0</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="32"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="33">
+        <v>23.0</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="23">
+        <v>24.0</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="16">
+        <v>25.0</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="23">
+        <v>26.0</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="33">
+        <v>27.0</v>
+      </c>
+      <c r="B34" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="H34" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" s="33"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="23">
+        <v>28.0</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="H35" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I35" s="32"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="16">
+        <v>29.0</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="23">
+        <v>30.0</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="32"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="33">
+        <v>31.0</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="23">
+        <v>32.0</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="56"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="16">
+        <v>33.0</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" s="33">
+        <v>14.0</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="23">
+        <v>34.0</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="32"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="33">
+        <v>35.0</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="71"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="23">
+        <v>36.0</v>
+      </c>
+      <c r="B43" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="H43" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="56"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="16">
+        <v>37.0</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="23">
+        <v>38.0</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D45" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="H45" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="49"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="33">
+        <v>39.0</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="73">
+        <v>7.3412011E8</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G46" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="H46" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="23">
+        <v>40.0</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="F47" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="H47" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="49"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="16">
+        <v>41.0</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="G48" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="H48" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="23">
+        <v>42.0</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" s="76">
+        <v>1.0</v>
+      </c>
+      <c r="D49" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="F49" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="23"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="33">
+        <v>43.0</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G50" s="69" t="s">
+        <v>214</v>
+      </c>
+      <c r="H50" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="23">
+        <v>44.0</v>
+      </c>
+      <c r="B51" s="51" t="s">
+        <v>274</v>
+      </c>
+      <c r="C51" s="49">
+        <v>8.0</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="E51" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="F51" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="G51" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="56"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="16">
+        <v>45.0</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="C52" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="69" t="s">
+        <v>222</v>
+      </c>
+      <c r="H52" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" s="16"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="23">
+        <v>46.0</v>
+      </c>
+      <c r="B53" s="56"/>
+      <c r="C53" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="F53" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="49"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="33">
+        <v>47.0</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="16">
+        <v>12.0</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="23">
+        <v>48.0</v>
+      </c>
+      <c r="B55" s="51" t="s">
+        <v>276</v>
+      </c>
+      <c r="C55" s="49">
+        <v>4.0</v>
+      </c>
+      <c r="D55" s="49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E55" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="F55" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="G55" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="H55" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I55" s="49"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="16">
+        <v>49.0</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C56" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" s="22"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="23">
+        <v>50.0</v>
+      </c>
+      <c r="B57" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="C57" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D57" s="49" t="s">
+        <v>240</v>
+      </c>
+      <c r="E57" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="F57" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="G57" s="79" t="s">
+        <v>243</v>
+      </c>
+      <c r="H57" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" s="56"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="33">
+        <v>51.0</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I58" s="38"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="23">
+        <v>52.0</v>
+      </c>
+      <c r="B59" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="C59" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="F59" s="49" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="H59" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I59" s="56"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="16">
+        <v>53.0</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E60" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="72" t="s">
+      <c r="F60" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G60" s="69" t="s">
         <v>256</v>
       </c>
-      <c r="G7" s="72" t="s">
-        <v>257</v>
-      </c>
-      <c r="H7" s="72" t="s">
-        <v>258</v>
-      </c>
-      <c r="I7" s="72" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="73">
-        <v>1.0</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="74" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="58"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="75">
-        <v>2.0</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="C9" s="76" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="76" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="77"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="73">
-        <v>3.0</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>261</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>263</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>264</v>
-      </c>
-      <c r="G10" s="53" t="s">
-        <v>265</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="I10" s="58"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="75">
-        <v>4.0</v>
-      </c>
-      <c r="B11" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="77"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="73">
-        <v>5.0</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>260</v>
-      </c>
-      <c r="C12" s="74" t="s">
-        <v>266</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>267</v>
-      </c>
-      <c r="F12" s="53" t="s">
-        <v>268</v>
-      </c>
-      <c r="G12" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="58"/>
+      <c r="H60" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I60" s="22"/>
     </row>
     <row r="100">
-      <c r="T100" s="78" t="s">
-        <v>270</v>
+      <c r="T100" s="87" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>